<commit_message>
ajuste año y mes
</commit_message>
<xml_diff>
--- a/data/metas/Metas nov.xlsx
+++ b/data/metas/Metas nov.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vladimir\Documents\Reportes\track\TRACK BI\data\metas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C41EFB5B-B38E-415E-8ADE-AB539EEF9CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D1E149-2453-401A-B8C9-EFCC85EA01E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15696" xr2:uid="{25CE6252-27A9-4B41-ABF1-E4554C54E68E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>VILLAS DEL REY</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Meta de clientes nuevos</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Mes</t>
   </si>
 </sst>
 </file>
@@ -134,7 +140,7 @@
     <numFmt numFmtId="164" formatCode="_-[$$-80A]* #,##0_-;\-[$$-80A]* #,##0_-;_-[$$-80A]* &quot;-&quot;??_-;_-@"/>
     <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,23 +149,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -173,102 +166,21 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFFC000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FFFFC000"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -306,64 +218,27 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -658,9 +533,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{270C0CE8-2C9D-4E45-89F3-304CDC43FD91}" name="Tabla1" displayName="Tabla1" ref="A2:H24" totalsRowShown="0" tableBorderDxfId="8">
-  <autoFilter ref="A2:H24" xr:uid="{270C0CE8-2C9D-4E45-89F3-304CDC43FD91}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{270C0CE8-2C9D-4E45-89F3-304CDC43FD91}" name="Tabla1" displayName="Tabla1" ref="A2:J24" totalsRowShown="0" tableBorderDxfId="8">
+  <autoFilter ref="A2:J24" xr:uid="{270C0CE8-2C9D-4E45-89F3-304CDC43FD91}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{77AEC5E1-75A8-4D26-B7C6-FEB178F6E1C1}" name="Sucursales" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{7462DAAF-6DB4-4405-8508-73A33ADDFB4F}" name="Meta FAYCGO " dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{26715BA0-E2DF-41F2-B9B9-1F62E0CE5131}" name="Usuarios 1ro de mes" dataDxfId="5"/>
@@ -675,6 +550,8 @@
     <tableColumn id="8" xr3:uid="{70BCCEC0-77FB-4C5B-A333-BAA74285D0C7}" name="Tienda" dataDxfId="0">
       <calculatedColumnFormula>F3+G3</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="9" xr3:uid="{5072CA0F-EA14-4D3C-A062-1A5ABD714150}" name="Año"/>
+    <tableColumn id="10" xr3:uid="{1F63E2B1-9C9F-411C-903A-4ADC7A6B9DA9}" name="Mes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -977,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404D95DA-BDF5-4CE9-B38E-D0639C2B77E5}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A2:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,669 +873,806 @@
     <col min="9" max="10" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:8" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="1">
         <v>784027</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="2">
         <v>1285</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>1279</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="2">
         <v>153</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="4">
         <f>B3*0.07</f>
         <v>54881.890000000007</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="5">
         <f>(B3*0.013)</f>
         <v>10192.350999999999</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="6">
         <f>F3+G3</f>
         <v>65074.241000000009</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="I3">
+        <v>2025</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="1">
         <v>679130</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <v>1159</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="3">
         <v>1130</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="2">
         <v>81</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="4">
         <f t="shared" ref="F4:F24" si="0">B4*0.07</f>
         <v>47539.100000000006</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="5">
         <f t="shared" ref="G4:G24" si="1">(B4*0.013)</f>
         <v>8828.6899999999987</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="6">
         <f t="shared" ref="H4:H24" si="2">F4+G4</f>
         <v>56367.790000000008</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="I4">
+        <v>2025</v>
+      </c>
+      <c r="J4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="1">
         <v>840360</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="2">
         <v>1425</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <v>1410</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="2">
         <v>106</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="4">
         <f t="shared" si="0"/>
         <v>58825.200000000004</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="5">
         <f t="shared" si="1"/>
         <v>10924.68</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="6">
         <f t="shared" si="2"/>
         <v>69749.88</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="I5">
+        <v>2025</v>
+      </c>
+      <c r="J5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="1">
         <v>795739</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <v>1337</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>1351</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="2">
         <v>107</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="4">
         <f t="shared" si="0"/>
         <v>55701.73</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="5">
         <f t="shared" si="1"/>
         <v>10344.607</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="6">
         <f t="shared" si="2"/>
         <v>66046.337</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="I6">
+        <v>2025</v>
+      </c>
+      <c r="J6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="1">
         <v>1124040</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="2">
         <v>1952</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <v>1938</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="2">
         <v>158</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="4">
         <f t="shared" si="0"/>
         <v>78682.8</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="5">
         <f t="shared" si="1"/>
         <v>14612.519999999999</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="6">
         <f t="shared" si="2"/>
         <v>93295.32</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="I7">
+        <v>2025</v>
+      </c>
+      <c r="J7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>743862</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="2">
         <v>1261</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="3">
         <v>1246</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="2">
         <v>115</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="4">
         <f t="shared" si="0"/>
         <v>52070.340000000004</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="5">
         <f t="shared" si="1"/>
         <v>9670.2060000000001</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="6">
         <f t="shared" si="2"/>
         <v>61740.546000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="I8">
+        <v>2025</v>
+      </c>
+      <c r="J8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>668627</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <v>1043</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="3">
         <v>1063</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="2">
         <v>170</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="4">
         <f t="shared" si="0"/>
         <v>46803.890000000007</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="5">
         <f t="shared" si="1"/>
         <v>8692.1509999999998</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="6">
         <f t="shared" si="2"/>
         <v>55496.041000000005</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="I9">
+        <v>2025</v>
+      </c>
+      <c r="J9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="1">
         <v>936600</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="2">
         <v>1682</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="3">
         <v>1561</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="2">
         <v>126</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="4">
         <f t="shared" si="0"/>
         <v>65562</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="5">
         <f t="shared" si="1"/>
         <v>12175.8</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="6">
         <f t="shared" si="2"/>
         <v>77737.8</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+      <c r="I10">
+        <v>2025</v>
+      </c>
+      <c r="J10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="1">
         <v>1595392</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="2">
         <v>2466</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="3">
         <v>2432</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="2">
         <v>258</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="4">
         <f t="shared" si="0"/>
         <v>111677.44000000002</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="5">
         <f t="shared" si="1"/>
         <v>20740.095999999998</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="6">
         <f t="shared" si="2"/>
         <v>132417.53600000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
+      <c r="I11">
+        <v>2025</v>
+      </c>
+      <c r="J11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="1">
         <v>402441</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="2">
         <v>653</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="3">
         <v>663</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="2">
         <v>97</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="4">
         <f t="shared" si="0"/>
         <v>28170.870000000003</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="5">
         <f t="shared" si="1"/>
         <v>5231.7330000000002</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="6">
         <f t="shared" si="2"/>
         <v>33402.603000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="I12">
+        <v>2025</v>
+      </c>
+      <c r="J12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="1">
         <v>1132285</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="2">
         <v>1935</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="3">
         <v>1903</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="2">
         <v>177</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="4">
         <f t="shared" si="0"/>
         <v>79259.950000000012</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="5">
         <f t="shared" si="1"/>
         <v>14719.705</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="6">
         <f t="shared" si="2"/>
         <v>93979.655000000013</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4">
+      <c r="I13">
+        <v>2025</v>
+      </c>
+      <c r="J13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1">
         <v>1092854</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="2">
         <v>1785</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="3">
         <v>1757</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="2">
         <v>164</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="4">
         <f t="shared" si="0"/>
         <v>76499.780000000013</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="5">
         <f t="shared" si="1"/>
         <v>14207.101999999999</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="6">
         <f t="shared" si="2"/>
         <v>90706.882000000012</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+      <c r="I14">
+        <v>2025</v>
+      </c>
+      <c r="J14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="1">
         <v>759536</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="2">
         <v>1214</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="3">
         <v>1283</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="2">
         <v>132</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="4">
         <f t="shared" si="0"/>
         <v>53167.520000000004</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="5">
         <f t="shared" si="1"/>
         <v>9873.9679999999989</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="6">
         <f t="shared" si="2"/>
         <v>63041.488000000005</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
+      <c r="I15">
+        <v>2025</v>
+      </c>
+      <c r="J15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="1">
         <v>877058</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="2">
         <v>1602</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="3">
         <v>1586</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="2">
         <v>120</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="4">
         <f t="shared" si="0"/>
         <v>61394.060000000005</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="5">
         <f t="shared" si="1"/>
         <v>11401.753999999999</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="6">
         <f t="shared" si="2"/>
         <v>72795.813999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
+      <c r="I16">
+        <v>2025</v>
+      </c>
+      <c r="J16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="1">
         <v>848085</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="2">
         <v>1450</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="3">
         <v>1435</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="2">
         <v>116</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="4">
         <f t="shared" si="0"/>
         <v>59365.950000000004</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="5">
         <f t="shared" si="1"/>
         <v>11025.105</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="6">
         <f t="shared" si="2"/>
         <v>70391.055000000008</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+      <c r="I17">
+        <v>2025</v>
+      </c>
+      <c r="J17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="1">
         <v>693528</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="2">
         <v>1258</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="3">
         <v>1221</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="2">
         <v>101</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="4">
         <f t="shared" si="0"/>
         <v>48546.960000000006</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="5">
         <f t="shared" si="1"/>
         <v>9015.8639999999996</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="6">
         <f t="shared" si="2"/>
         <v>57562.824000000008</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="I18">
+        <v>2025</v>
+      </c>
+      <c r="J18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="1">
         <v>604128</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="2">
         <v>1016</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="3">
         <v>992</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="2">
         <v>106</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="4">
         <f t="shared" si="0"/>
         <v>42288.960000000006</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="5">
         <f t="shared" si="1"/>
         <v>7853.6639999999998</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="6">
         <f t="shared" si="2"/>
         <v>50142.624000000003</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
+      <c r="I19">
+        <v>2025</v>
+      </c>
+      <c r="J19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="1">
         <v>1107792</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="2">
         <v>1765</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="3">
         <v>1764</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="2">
         <v>155</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="4">
         <f t="shared" si="0"/>
         <v>77545.440000000002</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="5">
         <f t="shared" si="1"/>
         <v>14401.295999999998</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="6">
         <f t="shared" si="2"/>
         <v>91946.736000000004</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
+      <c r="I20">
+        <v>2025</v>
+      </c>
+      <c r="J20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="1">
         <v>598484</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="2">
         <v>912</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="3">
         <v>953</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="2">
         <v>129</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="4">
         <f t="shared" si="0"/>
         <v>41893.880000000005</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="5">
         <f t="shared" si="1"/>
         <v>7780.2919999999995</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="6">
         <f t="shared" si="2"/>
         <v>49674.172000000006</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
+      <c r="I21">
+        <v>2025</v>
+      </c>
+      <c r="J21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="1">
         <v>808264</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="2">
         <v>1427</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="3">
         <v>1423</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="2">
         <v>142</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="4">
         <f t="shared" si="0"/>
         <v>56578.48</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="5">
         <f t="shared" si="1"/>
         <v>10507.431999999999</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="6">
         <f t="shared" si="2"/>
         <v>67085.911999999997</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
+      <c r="I22">
+        <v>2025</v>
+      </c>
+      <c r="J22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="1">
         <v>789960</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="2">
         <v>1168</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="3">
         <v>1160</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="2">
         <v>115</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="4">
         <f t="shared" si="0"/>
         <v>55297.200000000004</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="5">
         <f t="shared" si="1"/>
         <v>10269.48</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="6">
         <f t="shared" si="2"/>
         <v>65566.680000000008</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
+      <c r="I23">
+        <v>2025</v>
+      </c>
+      <c r="J23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="1">
         <v>961074</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="2">
         <v>1273</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="3">
         <v>1497</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="2">
         <v>315</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="4">
         <f t="shared" si="0"/>
         <v>67275.180000000008</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="5">
         <f t="shared" si="1"/>
         <v>12493.962</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="6">
         <f t="shared" si="2"/>
         <v>79769.142000000007</v>
+      </c>
+      <c r="I24">
+        <v>2025</v>
+      </c>
+      <c r="J24">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>